<commit_message>
production environment 20221003 10511645
</commit_message>
<xml_diff>
--- a/OnCall/2022-08-22 to 2022-08-29/On Call Report.xlsx
+++ b/OnCall/2022-08-22 to 2022-08-29/On Call Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIP\OnCall\2022-08-22 to 2022-08-29\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\WIP\OnCall\2022-08-22 to 2022-08-29\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF32433B-0818-4195-8707-DF24DA2DDC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC44DBBC-4EDD-47F5-9287-54C69BB00E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="-16470" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{811B3618-D1A8-47C6-AF60-49222DFFA8E5}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{811B3618-D1A8-47C6-AF60-49222DFFA8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Job Failures" sheetId="1" r:id="rId1"/>
@@ -661,20 +661,20 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="172.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="172.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -714,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -770,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -804,7 +804,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -830,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1208,12 +1208,12 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="118.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="118.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1310,20 +1310,20 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>11584</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>11569</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>11577</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>11589</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>17</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>11603</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>21</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>11573</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>11606</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>11578</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>11575</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>11579</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>11590</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>11604</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>11592</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>11582</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>11574</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>11585</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>11602</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>11572</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>24</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>11605</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>11570</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>11580</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>11581</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>11591</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>11571</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
production environment 20221003 1053
</commit_message>
<xml_diff>
--- a/OnCall/2022-08-22 to 2022-08-29/On Call Report.xlsx
+++ b/OnCall/2022-08-22 to 2022-08-29/On Call Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\WIP\OnCall\2022-08-22 to 2022-08-29\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC44DBBC-4EDD-47F5-9287-54C69BB00E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD37BA09-5DF5-49C0-A2F7-04C12EF15BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{811B3618-D1A8-47C6-AF60-49222DFFA8E5}"/>
+    <workbookView xWindow="780" yWindow="870" windowWidth="21630" windowHeight="11295" activeTab="2" xr2:uid="{811B3618-D1A8-47C6-AF60-49222DFFA8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Job Failures" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="109">
   <si>
     <t>SQL08</t>
   </si>
@@ -90,9 +90,6 @@
     <t>SentryOne.dbo.EventSourceHistory; SentryOne.dbo.MetaHistorySqlServerTraceLog</t>
   </si>
   <si>
-    <t>SysproCompany100.dbo.SorMaster</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t xml:space="preserve"> 7SYSPRO; Microsoft Office 2013 (victim)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 7SYSPRO; 1-MN-SC2065-PC (victim)</t>
-  </si>
-  <si>
     <t>WarehouseCompany100.dbo.tblPalletItem; WarehouseCompany100.dbo.tblPalletReserved</t>
   </si>
   <si>
@@ -240,55 +234,136 @@
     <t xml:space="preserve"> SQL Beacon Agent Gen2 (victim); SQLAgent - TSQL JobStep (Job 0xAB9A1F5B02FDDD4EAF8A08B09C40948E : Step 1)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 7SYSPRO (victim); 7SYSPRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DWAYNEP_SYSPRO (victim); @WJR_SYSPRO</t>
-  </si>
-  <si>
     <t>SysproCompany100.dbo.SorDetail</t>
   </si>
   <si>
-    <t xml:space="preserve"> DS-HELEND; DSWIPPOST_SYSPRO (victim)</t>
-  </si>
-  <si>
-    <t>SysproCompany100.dbo.InvCompanyCtl; SysproCompany100.dbo.WipMaster</t>
-  </si>
-  <si>
     <t>tempdb.sys.sysschobjs</t>
   </si>
   <si>
-    <t xml:space="preserve"> DEV-THESG (victim); SQL08</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SUMMERCLASSICS\SentryOneUser (victim); SUMMERCLASSICS\SqlAgentUser</t>
-  </si>
-  <si>
-    <t>msdb.dbo.sysjobhistory</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DS-AUBREYG; DS-ZANQUESEJ (victim)</t>
-  </si>
-  <si>
-    <t>SysproCompany100.dbo.SorDetailBin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DS-ZANQUESEJ; DSWIPPOST_SYSPRO (victim)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DS-DAVERINB; SUMMERCLASSICS\DeDeH (victim)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7SYSPRO; 1-MV-SC2324-LTP (victim)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DS-HUNTERD; SUMMERCLASSICS\MichelleW (victim)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WMS</t>
-  </si>
-  <si>
-    <t>WarehouseCompany100.dbo.tblPalletReservedArchive</t>
+    <t xml:space="preserve"> 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DS-TREZMANH</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.InvWarehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Microsoft SQL Server Management Studio - Query (victim); SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-MN-SC2909-PC (victim); 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\Ben (victim); HASSIET_SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLAgent - TSQL JobStep (Job 0xA08E18747DB4E945896AEBE75F59E191 : Step 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLREPORTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\Svc_SQL_DE</t>
+  </si>
+  <si>
+    <t>Reports.dbo.rt_Sub_DataDrivenLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUGARCRM_UPSERT (victim); SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TALEND (victim); 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQL_Talend (victim); ASHLIEW_SYSPRO</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.CusSorMaster+; SysproCompany100.dbo.SorMaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SYSPRO; SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STEPHANIET_SYSPRO; ALYSSAC_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.GenJournalDetail</t>
+  </si>
+  <si>
+    <t>WarehouseCompany100.dbo.tblPalletReserved; WarehouseCompany100.dbo.tblPickingSlipItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ENTERWORKSAPP; ENTERWORKSAPP (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EWsys; EWsys (victim)</t>
+  </si>
+  <si>
+    <t>EPX.dbo.P_WORK_ITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLAgent - TSQL JobStep (Job 0xB30BB317EFE6234FB5FC3C0BCAB00DD7 : Step 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARGARETH_SYSPRO; ASHLIEW_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.ArControl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Microsoft SQL Server Management Studio - Query (victim); SUMMERCLASSICS\EcatSalesOrderImport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEV-JUSTINP (victim); 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\adm_justinp (victim); SUMMERCLASSICS\EcatSalesOrderImport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLAgent - TSQL JobStep (Job 0x3AFC7C3496751340A2B761968B0E92A7 : Step 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLAgent - TSQL JobStep (Job 0xBF0C89C49B2416409AAD4489A1344C60 : Step 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STEPHANIET_SYSPRO; ELLENM_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DWAYNEP_SYSPRO; DS-ZANQUESEJ (victim)</t>
+  </si>
+  <si>
+    <t>WarehouseCompany100.dbo.tblPalletReserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Replication Distribution Agent; Tableau 2022.1 (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLREPORTING; DESKTOP-IGRF887 (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\SqlAgentUser; RJAYARAM (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.ArTrnSummary; SysproCompany100.dbo.SorMaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLAgent - TSQL JobStep (Job 0xA62A0F9C12F462478366837A3C4E2052 : Step 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\adm_ericc; SUMMERCLASSICS\SentryOneUser (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEV-THESG; SQLREPORTING (victim)</t>
+  </si>
+  <si>
+    <t>tempdb.dbo.#A010EBEC; tempdb.dbo.#BC405B08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUEB_SYSPRO; LEEE_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.GenControl</t>
   </si>
 </sst>
 </file>
@@ -684,7 +759,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -692,7 +767,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -700,7 +775,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -708,7 +783,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -716,7 +791,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -724,7 +799,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -732,7 +807,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -740,7 +815,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -748,7 +823,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -756,7 +831,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -764,7 +839,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -772,7 +847,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -780,7 +855,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -788,7 +863,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -832,10 +907,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -850,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s">
         <v>0</v>
@@ -858,10 +933,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -876,7 +951,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H19" t="s">
         <v>0</v>
@@ -884,10 +959,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -902,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
         <v>0</v>
@@ -910,10 +985,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -928,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
@@ -936,10 +1011,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -954,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -962,10 +1037,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -980,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" t="s">
         <v>0</v>
@@ -988,10 +1063,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1006,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -1014,10 +1089,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1032,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H25" t="s">
         <v>0</v>
@@ -1040,10 +1115,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1058,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H26" t="s">
         <v>0</v>
@@ -1066,10 +1141,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1084,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H27" t="s">
         <v>0</v>
@@ -1092,10 +1167,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1110,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H28" t="s">
         <v>0</v>
@@ -1118,10 +1193,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -1136,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
         <v>0</v>
@@ -1144,10 +1219,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1162,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30" t="s">
         <v>0</v>
@@ -1170,10 +1245,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1188,7 +1263,7 @@
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H31" t="s">
         <v>0</v>
@@ -1215,13 +1290,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1">
         <f>SUM(B2:B15)</f>
@@ -1230,7 +1305,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1238,7 +1313,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1246,7 +1321,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1254,7 +1329,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1262,7 +1337,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1270,7 +1345,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1294,7 +1369,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1307,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A7C9C2-741E-4F4E-A66D-EB086C7FF489}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,25 +1400,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1351,10 +1426,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <v>44797.523279976849</v>
+        <v>44834.563924108799</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>67</v>
@@ -1366,7 +1441,7 @@
         <v>69</v>
       </c>
       <c r="G2">
-        <v>11584</v>
+        <v>12885</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1374,22 +1449,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="6">
-        <v>44795.448156944447</v>
+        <v>44830.632940243057</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>11569</v>
+        <v>12861</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1397,7 +1472,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="6">
-        <v>44796.376856365743</v>
+        <v>44832.565205937499</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1409,10 +1484,10 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G4">
-        <v>11577</v>
+        <v>12874</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1420,7 +1495,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="6">
-        <v>44798.376645868055</v>
+        <v>44834.556142789355</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1432,10 +1507,10 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G5">
-        <v>11589</v>
+        <v>12884</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1443,22 +1518,22 @@
         <v>17</v>
       </c>
       <c r="B6" s="6">
-        <v>44799.573369907404</v>
+        <v>44831.503006944447</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="G6">
-        <v>11603</v>
+        <v>12866</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1466,22 +1541,22 @@
         <v>21</v>
       </c>
       <c r="B7" s="6">
-        <v>44795.902665243055</v>
+        <v>44833.312913113426</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="G7">
-        <v>11573</v>
+        <v>12879</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1489,76 +1564,76 @@
         <v>25</v>
       </c>
       <c r="B8" s="6">
-        <v>44801.166740277775</v>
+        <v>44832.458976122682</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>11606</v>
+        <v>12871</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6">
-        <v>44796.385694525467</v>
+        <v>44830.694514849536</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G9">
-        <v>11578</v>
+        <v>12863</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" s="6">
-        <v>44796.302406678238</v>
+        <v>44830.377649074071</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="G10">
-        <v>11575</v>
+        <v>12858</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="6">
-        <v>44796.41922329861</v>
+        <v>44832.473534143515</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1573,15 +1648,15 @@
         <v>12</v>
       </c>
       <c r="G11">
-        <v>11579</v>
+        <v>12872</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6">
-        <v>44798.555531747683</v>
+        <v>44834.551571412034</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -1593,41 +1668,41 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="G12">
-        <v>11590</v>
+        <v>12882</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="6">
-        <v>44799.600465972224</v>
+        <v>44833.438969710645</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="G13">
-        <v>11604</v>
+        <v>12880</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6">
-        <v>44798.752589583331</v>
+        <v>44830.317726655092</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1642,61 +1717,61 @@
         <v>16</v>
       </c>
       <c r="G14">
-        <v>11592</v>
+        <v>12857</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6">
-        <v>44796.583163854164</v>
+        <v>44833.312804247682</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="G15">
-        <v>11582</v>
+        <v>12876</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B16" s="6">
-        <v>44796.294901307869</v>
+        <v>44830.618995983794</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="G16">
-        <v>11574</v>
+        <v>12860</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B17" s="6">
-        <v>44797.591468402781</v>
+        <v>44830.377735960647</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1708,18 +1783,18 @@
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G17">
-        <v>11585</v>
+        <v>12859</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B18" s="6">
-        <v>44799.391578854164</v>
+        <v>44832.492029398149</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1731,194 +1806,309 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="G18">
-        <v>11602</v>
+        <v>12873</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B19" s="6">
-        <v>44795.763246180555</v>
+        <v>44834.556084837961</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="G19">
-        <v>11572</v>
+        <v>12883</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B20" s="6">
-        <v>44800.233118402779</v>
+        <v>44832.383314733794</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
+        <v>93</v>
+      </c>
+      <c r="F20">
+        <v>-1305762798</v>
       </c>
       <c r="G20">
-        <v>11605</v>
+        <v>12869</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6">
-        <v>44795.612785567129</v>
+        <v>44833.312862037033</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="G21">
-        <v>11570</v>
+        <v>12877</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B22" s="6">
-        <v>44796.433161805558</v>
+        <v>44832.312646180559</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G22">
-        <v>11580</v>
+        <v>12868</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B23" s="6">
-        <v>44796.520770682873</v>
+        <v>44830.694456793979</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="G23">
-        <v>11581</v>
+        <v>12862</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B24" s="6">
-        <v>44798.726654398146</v>
+        <v>44831.579732986109</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G24">
-        <v>11591</v>
+        <v>12867</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B25" s="6">
-        <v>44795.651819247687</v>
+        <v>44832.454831053241</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="G25">
-        <v>11571</v>
+        <v>12870</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B26" s="6">
-        <v>44798.776962581018</v>
+        <v>44833.456100659721</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26">
+        <v>12881</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>14</v>
       </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26">
-        <v>11593</v>
+      <c r="B27" s="6">
+        <v>44831.488245636574</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27">
+        <v>12865</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>18</v>
+      </c>
+      <c r="B28" s="6">
+        <v>44831.342117708336</v>
+      </c>
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28">
+        <v>12864</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="6">
+        <v>44833.312891203706</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29">
+        <v>12878</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" s="6">
+        <v>44835.208468900462</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30">
+        <v>12886</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6">
+        <v>44832.574637997684</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31">
+        <v>12875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>